<commit_message>
bug fixed, recording speed is more faster than before, unused code removed
</commit_message>
<xml_diff>
--- a/src/test/files/link_data.xlsx
+++ b/src/test/files/link_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -28,13 +28,10 @@
     <t xml:space="preserve">Links</t>
   </si>
   <si>
-    <t xml:space="preserve">17:26:00</t>
+    <t xml:space="preserve">17:35:00</t>
   </si>
   <si>
     <t xml:space="preserve">Sjt-fdxr-mnk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:27:00</t>
   </si>
   <si>
     <t xml:space="preserve">Hwy-gain-zbq</t>
@@ -167,10 +164,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
   </cols>
@@ -193,18 +190,18 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>